<commit_message>
merged files for 2015-02-02
</commit_message>
<xml_diff>
--- a/Upgrade6.0.xlsx
+++ b/Upgrade6.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="34935" windowHeight="16620"/>
+    <workbookView xWindow="300" yWindow="105" windowWidth="27270" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Upgrade6.0" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2897" uniqueCount="1454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2920" uniqueCount="1464">
   <si>
     <t>Processing diffs for the following: /cygdrive/c/Users/ronald/bin/rrgUpgrade60.sh -c /cygdrive/c/Users/ronald/uh-kc-customizations-5.1/src -o /cygdrive/c/Users/ronald/uh-kc-5.1/kc_project/src -r /cygdrive/c/Users/ronald/uh-kc-rice-5.1 -n /cygdrive/c/Users/ronald/github/UhKc/ -a /cygdrive/c/Users/ronald/github/uh-kc-api/coeus-api-all</t>
   </si>
@@ -4434,10 +4434,41 @@
     <t>KC-166 Change reject button UH specific to return for changes button</t>
   </si>
   <si>
-    <t>Rework-Rename button reject to return for changes….It's somewhere else in this code</t>
-  </si>
-  <si>
     <t>Assign to MikeB</t>
+  </si>
+  <si>
+    <t>Removed - Kuali made same change</t>
+  </si>
+  <si>
+    <t>KC-729 Make YNQ Questions not required in Organization Maintenance</t>
+  </si>
+  <si>
+    <t>coeus-impl/src/main/java/org/kuali/coeus/common/impl/org/OrganizationMaintenanceDocumentRule.java</t>
+  </si>
+  <si>
+    <t>Removed - File was renamed but once I found the file mergetool revealed our code change is in KC60 new version of this base class</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KC-765 BEGIN Project Title error passes validation, but prevents document from being submitted to sponsor
+New File name is KcTransactionalDocumentRuleBase.java</t>
+  </si>
+  <si>
+    <t>Review-Rework-Rename button reject to return for changes….It's somewhere else in this code</t>
+  </si>
+  <si>
+    <t>Images Keep</t>
+  </si>
+  <si>
+    <t>coeus-webapp/src/main/webapp/static/uh-images</t>
+  </si>
+  <si>
+    <t>KC-763 Validation throws exception if proposal is s2s and AOR has no address configured.</t>
+  </si>
+  <si>
+    <t>Merged-File Moved to s2s project</t>
+  </si>
+  <si>
+    <t>coeus-s2sgen-impl/src/main/java/org/kuali/coeus/s2sgen/impl/generate/support/GlobalLibraryV2_0Generator.java</t>
   </si>
 </sst>
 </file>
@@ -5292,10 +5323,10 @@
   <dimension ref="A1:M320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="F126" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="D155" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="F130" sqref="F130"/>
+      <selection pane="bottomRight" activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.140625" defaultRowHeight="15"/>
@@ -5348,14 +5379,14 @@
       </c>
       <c r="F6" s="5">
         <f>COUNTA(I13:I400)-COUNTIF(I13:I400," ")</f>
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="H6" t="s">
         <v>1234</v>
       </c>
       <c r="I6" s="3">
         <f>COUNTIF(I13:I400,"Merged*")</f>
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -5371,14 +5402,14 @@
       </c>
       <c r="F7" s="5">
         <f>F6/C10</f>
-        <v>0.9732142857142857</v>
+        <v>1.1785714285714286</v>
       </c>
       <c r="H7" t="s">
         <v>1235</v>
       </c>
       <c r="I7" s="3">
         <f>COUNTIF(I13:I400,"Keep*")</f>
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5394,14 +5425,14 @@
       </c>
       <c r="F8" s="5">
         <f>COUNTIF(I13:I400,"REVIEW*")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
         <v>1378</v>
       </c>
       <c r="I8" s="3">
         <f>COUNTIF(I13:I400,"Removed*")</f>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5417,14 +5448,14 @@
       </c>
       <c r="F9" s="5">
         <f>F8/C10</f>
-        <v>8.9285714285714288E-2</v>
+        <v>9.8214285714285712E-2</v>
       </c>
       <c r="H9" t="s">
         <v>1365</v>
       </c>
       <c r="I9" s="3">
         <f>COUNTIF(I13:I400,"REVIEW*")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5440,7 +5471,7 @@
       </c>
       <c r="I10" s="3">
         <f>SUM(I6:I9)</f>
-        <v>107</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -9603,7 +9634,7 @@
         <v>42034</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>1452</v>
+        <v>1458</v>
       </c>
       <c r="J129" s="3" t="s">
         <v>1451</v>
@@ -9615,10 +9646,10 @@
         <v>1245</v>
       </c>
       <c r="M129" t="s">
-        <v>1453</v>
-      </c>
-    </row>
-    <row r="130" spans="1:13">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" ht="30">
       <c r="A130" t="s">
         <v>23</v>
       </c>
@@ -9640,17 +9671,23 @@
       <c r="G130" s="5" t="s">
         <v>529</v>
       </c>
-      <c r="H130" t="s">
-        <v>29</v>
+      <c r="H130" s="7">
+        <v>42037</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>29</v>
+        <v>1453</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>1381</v>
+      </c>
+      <c r="K130" t="s">
+        <v>1245</v>
       </c>
       <c r="L130" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" ht="45">
       <c r="A131" t="s">
         <v>23</v>
       </c>
@@ -9672,17 +9709,23 @@
       <c r="G131" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="H131" t="s">
-        <v>29</v>
+      <c r="H131" s="7">
+        <v>42037</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>29</v>
+        <v>1234</v>
+      </c>
+      <c r="J131" s="3" t="s">
+        <v>1454</v>
+      </c>
+      <c r="K131" t="s">
+        <v>1455</v>
       </c>
       <c r="L131" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="105">
       <c r="A132" t="s">
         <v>223</v>
       </c>
@@ -9701,17 +9744,23 @@
       <c r="G132" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="H132" t="s">
-        <v>29</v>
+      <c r="H132" s="7">
+        <v>42037</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>29</v>
+        <v>1456</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>1457</v>
+      </c>
+      <c r="K132" t="s">
+        <v>1245</v>
       </c>
       <c r="L132" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="45">
       <c r="A133" t="s">
         <v>223</v>
       </c>
@@ -9730,14 +9779,20 @@
       <c r="G133" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="H133" t="s">
-        <v>29</v>
+      <c r="H133" s="7">
+        <v>42037</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>29</v>
+        <v>1462</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>1461</v>
+      </c>
+      <c r="K133" t="s">
+        <v>1463</v>
       </c>
       <c r="L133" t="s">
-        <v>29</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="134" spans="1:13">
@@ -12117,11 +12172,17 @@
       <c r="G218" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="H218" t="s">
-        <v>29</v>
+      <c r="H218" s="7">
+        <v>42037</v>
       </c>
       <c r="I218" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J218" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K218" t="s">
+        <v>1460</v>
       </c>
       <c r="L218" t="s">
         <v>29</v>
@@ -12143,11 +12204,17 @@
       <c r="G219" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="H219" t="s">
-        <v>29</v>
+      <c r="H219" s="7">
+        <v>42037</v>
       </c>
       <c r="I219" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J219" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K219" t="s">
+        <v>1460</v>
       </c>
       <c r="L219" t="s">
         <v>29</v>
@@ -12169,11 +12236,17 @@
       <c r="G220" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="H220" t="s">
-        <v>29</v>
+      <c r="H220" s="7">
+        <v>42037</v>
       </c>
       <c r="I220" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J220" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K220" t="s">
+        <v>1460</v>
       </c>
       <c r="L220" t="s">
         <v>29</v>
@@ -12195,11 +12268,17 @@
       <c r="G221" s="5" t="s">
         <v>860</v>
       </c>
-      <c r="H221" t="s">
-        <v>29</v>
+      <c r="H221" s="7">
+        <v>42037</v>
       </c>
       <c r="I221" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J221" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K221" t="s">
+        <v>1460</v>
       </c>
       <c r="L221" t="s">
         <v>29</v>
@@ -12221,11 +12300,17 @@
       <c r="G222" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="H222" t="s">
-        <v>29</v>
+      <c r="H222" s="7">
+        <v>42037</v>
       </c>
       <c r="I222" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J222" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K222" t="s">
+        <v>1460</v>
       </c>
       <c r="L222" t="s">
         <v>29</v>
@@ -12247,11 +12332,17 @@
       <c r="G223" s="5" t="s">
         <v>866</v>
       </c>
-      <c r="H223" t="s">
-        <v>29</v>
+      <c r="H223" s="7">
+        <v>42037</v>
       </c>
       <c r="I223" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J223" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K223" t="s">
+        <v>1460</v>
       </c>
       <c r="L223" t="s">
         <v>29</v>
@@ -12273,11 +12364,17 @@
       <c r="G224" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="H224" t="s">
-        <v>29</v>
+      <c r="H224" s="7">
+        <v>42037</v>
       </c>
       <c r="I224" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J224" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K224" t="s">
+        <v>1460</v>
       </c>
       <c r="L224" t="s">
         <v>29</v>
@@ -12299,11 +12396,17 @@
       <c r="G225" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="H225" t="s">
-        <v>29</v>
+      <c r="H225" s="7">
+        <v>42037</v>
       </c>
       <c r="I225" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J225" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K225" t="s">
+        <v>1460</v>
       </c>
       <c r="L225" t="s">
         <v>29</v>
@@ -12325,11 +12428,17 @@
       <c r="G226" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="H226" t="s">
-        <v>29</v>
+      <c r="H226" s="7">
+        <v>42037</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J226" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K226" t="s">
+        <v>1460</v>
       </c>
       <c r="L226" t="s">
         <v>29</v>
@@ -12351,11 +12460,17 @@
       <c r="G227" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="H227" t="s">
-        <v>29</v>
+      <c r="H227" s="7">
+        <v>42037</v>
       </c>
       <c r="I227" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J227" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K227" t="s">
+        <v>1460</v>
       </c>
       <c r="L227" t="s">
         <v>29</v>
@@ -12377,11 +12492,17 @@
       <c r="G228" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="H228" t="s">
-        <v>29</v>
+      <c r="H228" s="7">
+        <v>42037</v>
       </c>
       <c r="I228" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J228" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K228" t="s">
+        <v>1460</v>
       </c>
       <c r="L228" t="s">
         <v>29</v>
@@ -12403,11 +12524,17 @@
       <c r="G229" s="5" t="s">
         <v>884</v>
       </c>
-      <c r="H229" t="s">
-        <v>29</v>
+      <c r="H229" s="7">
+        <v>42037</v>
       </c>
       <c r="I229" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J229" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K229" t="s">
+        <v>1460</v>
       </c>
       <c r="L229" t="s">
         <v>29</v>
@@ -12429,11 +12556,17 @@
       <c r="G230" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="H230" t="s">
-        <v>29</v>
+      <c r="H230" s="7">
+        <v>42037</v>
       </c>
       <c r="I230" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J230" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K230" t="s">
+        <v>1460</v>
       </c>
       <c r="L230" t="s">
         <v>29</v>
@@ -12455,11 +12588,17 @@
       <c r="G231" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="H231" t="s">
-        <v>29</v>
+      <c r="H231" s="7">
+        <v>42037</v>
       </c>
       <c r="I231" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J231" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K231" t="s">
+        <v>1460</v>
       </c>
       <c r="L231" t="s">
         <v>29</v>
@@ -12481,11 +12620,17 @@
       <c r="G232" s="5" t="s">
         <v>893</v>
       </c>
-      <c r="H232" t="s">
-        <v>29</v>
+      <c r="H232" s="7">
+        <v>42037</v>
       </c>
       <c r="I232" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J232" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K232" t="s">
+        <v>1460</v>
       </c>
       <c r="L232" t="s">
         <v>29</v>
@@ -12507,11 +12652,17 @@
       <c r="G233" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="H233" t="s">
-        <v>29</v>
+      <c r="H233" s="7">
+        <v>42037</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J233" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K233" t="s">
+        <v>1460</v>
       </c>
       <c r="L233" t="s">
         <v>29</v>
@@ -12533,11 +12684,17 @@
       <c r="G234" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="H234" t="s">
-        <v>29</v>
+      <c r="H234" s="7">
+        <v>42037</v>
       </c>
       <c r="I234" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J234" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K234" t="s">
+        <v>1460</v>
       </c>
       <c r="L234" t="s">
         <v>29</v>
@@ -12559,11 +12716,17 @@
       <c r="G235" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="H235" t="s">
-        <v>29</v>
+      <c r="H235" s="7">
+        <v>42037</v>
       </c>
       <c r="I235" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J235" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K235" t="s">
+        <v>1460</v>
       </c>
       <c r="L235" t="s">
         <v>29</v>
@@ -12585,11 +12748,17 @@
       <c r="G236" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="H236" t="s">
-        <v>29</v>
+      <c r="H236" s="7">
+        <v>42037</v>
       </c>
       <c r="I236" s="3" t="s">
-        <v>29</v>
+        <v>1235</v>
+      </c>
+      <c r="J236" s="3" t="s">
+        <v>1459</v>
+      </c>
+      <c r="K236" t="s">
+        <v>1460</v>
       </c>
       <c r="L236" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
merges for 2015-02-23 (Merges done, real work starts now)
</commit_message>
<xml_diff>
--- a/Upgrade6.0.xlsx
+++ b/Upgrade6.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="1867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3184" uniqueCount="1878">
   <si>
     <t>Processing diffs for the following: /cygdrive/c/Users/ronald/bin/rrgUpgrade60.sh -c /cygdrive/c/Users/ronald/uh-kc-customizations-5.1/src -o /cygdrive/c/Users/ronald/uh-kc-5.1/kc_project/src -r /cygdrive/c/Users/ronald/uh-kc-rice-5.1 -n /cygdrive/c/Users/ronald/github/UhKc/ -a /cygdrive/c/Users/ronald/github/uh-kc-api/coeus-api-all</t>
   </si>
@@ -5768,6 +5768,50 @@
   </si>
   <si>
     <t>coeus-impl/src/main/java/org/kuali/coeus/propdev/impl/krms/PropDevJavaFunctionKrmsTermServiceImpl.java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC-625 Copy Proposal is not honoring the Lead Unit Selected
+KC-641 Not all questions are copying when copy proposal is set to include questions
+KC-466 BEGIN - sponsor deadline date and sponsor deadline type were made required fields on save so they need to be copied too
+KC-865 BEGIN inactive ynq questions should not be copied during copy proposal process
+</t>
+  </si>
+  <si>
+    <t>Merged- Needs more Review- Code we modifed has been removed.  We should test to see if this issue still exists.
+KC-625 (Code removed-test)
+KC-641 (Code removed-test)
+KC-865 (Code removed-test)</t>
+  </si>
+  <si>
+    <t>coeus-impl/src/main/java/org/kuali/coeus/propdev/impl/copy/ProposalCopyServiceImpl.java</t>
+  </si>
+  <si>
+    <t>KC-778 Change Attachment Notifications so they are sent to ORS only.</t>
+  </si>
+  <si>
+    <t>coeus-impl/src/main/java/org/kuali/coeus/propdev/impl/abstrct/ProposalDevelopmentAbstractsAttachmentsAction.java</t>
+  </si>
+  <si>
+    <t>KC-573 KC 5.1 submission of development proposal throws incident report
+KC-855 Add feature to Questionnaire for smart answers
+KC-785 Many of the "print" buttons on the Proposal Summary tab don't work and generate incident reports.  Solution taken from KC 5.2 code so this should not be needed after next upgrade</t>
+  </si>
+  <si>
+    <t>Review - Merged - KC-855 merge was not lining up in p4merge so I had to hand merge this code. (Also had to modify the code because they changed method return types)  NEEDS TESTING
+KC-785 removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KC-793 Correct wording for validation warnings exist message in PD and Award
+KC-666 BEGIN Remove question about seeing future approvals</t>
+  </si>
+  <si>
+    <t>coeus-impl/src/main/java/org/kuali/coeus/propdev/impl/action/ProposalDevelopmentActionsAction.java</t>
+  </si>
+  <si>
+    <t>KC-579 : KC 5.1 Proposal: REJECT from the "approver view" (or proposal summary screen) nothing happens - must go to proposal actions to complete</t>
+  </si>
+  <si>
+    <t>coeus-impl/src/main/java/org/kuali/coeus/propdev/impl/approve/ProposalDevelopmentApproverViewAction.java</t>
   </si>
 </sst>
 </file>
@@ -6623,10 +6667,10 @@
   <dimension ref="A1:M324"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="D118" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="E123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="H125" sqref="H125"/>
+      <selection pane="bottomRight" activeCell="M125" sqref="M125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.140625" defaultRowHeight="15"/>
@@ -6681,14 +6725,14 @@
       </c>
       <c r="F6" s="5">
         <f>COUNTA(I13:I400)-COUNTIF(I13:I400," ")</f>
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="H6" t="s">
         <v>1133</v>
       </c>
       <c r="I6" s="3">
         <f>COUNTIF(I13:I400,"Merged*")</f>
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -6704,7 +6748,7 @@
       </c>
       <c r="F7" s="5">
         <f>F6/C10</f>
-        <v>2.603448275862069</v>
+        <v>2.646551724137931</v>
       </c>
       <c r="H7" t="s">
         <v>1134</v>
@@ -6727,7 +6771,7 @@
       </c>
       <c r="F8" s="5">
         <f>COUNTIF(I13:I400,"REVIEW*")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
         <v>1276</v>
@@ -6750,14 +6794,14 @@
       </c>
       <c r="F9" s="5">
         <f>F8/C10</f>
-        <v>0.16379310344827586</v>
+        <v>0.17241379310344829</v>
       </c>
       <c r="H9" t="s">
         <v>1263</v>
       </c>
       <c r="I9" s="3">
         <f>COUNTIF(I13:I400,"REVIEW*")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -6773,7 +6817,7 @@
       </c>
       <c r="I10" s="3">
         <f>SUM(I6:I9)</f>
-        <v>302</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -10660,7 +10704,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" ht="240">
       <c r="A121" t="s">
         <v>23</v>
       </c>
@@ -10682,17 +10726,23 @@
       <c r="G121" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="H121" t="s">
-        <v>29</v>
-      </c>
-      <c r="I121" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L121" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="122" spans="1:12">
+      <c r="H121" s="7">
+        <v>42058</v>
+      </c>
+      <c r="I121" s="10" t="s">
+        <v>1868</v>
+      </c>
+      <c r="J121" s="3" t="s">
+        <v>1867</v>
+      </c>
+      <c r="K121" t="s">
+        <v>1869</v>
+      </c>
+      <c r="L121" s="5" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="45">
       <c r="A122" t="s">
         <v>23</v>
       </c>
@@ -10714,17 +10764,23 @@
       <c r="G122" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="H122" t="s">
-        <v>29</v>
+      <c r="H122" s="7">
+        <v>42058</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L122" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="123" spans="1:12">
+        <v>1133</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>1870</v>
+      </c>
+      <c r="K122" t="s">
+        <v>1871</v>
+      </c>
+      <c r="L122" s="5" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="180">
       <c r="A123" t="s">
         <v>23</v>
       </c>
@@ -10746,17 +10802,23 @@
       <c r="G123" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="H123" t="s">
-        <v>29</v>
-      </c>
-      <c r="I123" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L123" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12">
+      <c r="H123" s="7">
+        <v>42058</v>
+      </c>
+      <c r="I123" s="10" t="s">
+        <v>1873</v>
+      </c>
+      <c r="J123" s="3" t="s">
+        <v>1872</v>
+      </c>
+      <c r="K123" t="s">
+        <v>1875</v>
+      </c>
+      <c r="L123" s="5" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="75">
       <c r="A124" t="s">
         <v>23</v>
       </c>
@@ -10778,17 +10840,23 @@
       <c r="G124" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="H124" t="s">
-        <v>29</v>
+      <c r="H124" s="7">
+        <v>42058</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L124" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="125" spans="1:12">
+        <v>1133</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>1874</v>
+      </c>
+      <c r="K124" t="s">
+        <v>1875</v>
+      </c>
+      <c r="L124" s="5" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="75">
       <c r="A125" t="s">
         <v>23</v>
       </c>
@@ -10804,20 +10872,26 @@
       <c r="E125" t="s">
         <v>502</v>
       </c>
-      <c r="F125" s="5" t="s">
+      <c r="F125" t="s">
         <v>503</v>
       </c>
-      <c r="G125" s="5" t="s">
+      <c r="G125" t="s">
         <v>504</v>
       </c>
-      <c r="H125" t="s">
-        <v>29</v>
-      </c>
-      <c r="I125" s="3" t="s">
-        <v>29</v>
+      <c r="H125">
+        <v>42058</v>
+      </c>
+      <c r="I125" t="s">
+        <v>1133</v>
+      </c>
+      <c r="J125" s="3" t="s">
+        <v>1876</v>
+      </c>
+      <c r="K125" t="s">
+        <v>1877</v>
       </c>
       <c r="L125" t="s">
-        <v>29</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="126" spans="1:12" ht="105">

</xml_diff>

<commit_message>
... Lastest version of Upgrade 6.0 excel sheet
</commit_message>
<xml_diff>
--- a/Upgrade6.0.xlsx
+++ b/Upgrade6.0.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="180" windowWidth="35805" windowHeight="16110"/>
+    <workbookView xWindow="180" yWindow="225" windowWidth="32220" windowHeight="16065" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Upgrade6.0" sheetId="1" r:id="rId1"/>
+    <sheet name="Change Made Directly to UH_KC" sheetId="2" r:id="rId2"/>
+    <sheet name="Rice Changes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3184" uniqueCount="1878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3425" uniqueCount="2021">
   <si>
     <t>Processing diffs for the following: /cygdrive/c/Users/ronald/bin/rrgUpgrade60.sh -c /cygdrive/c/Users/ronald/uh-kc-customizations-5.1/src -o /cygdrive/c/Users/ronald/uh-kc-5.1/kc_project/src -r /cygdrive/c/Users/ronald/uh-kc-rice-5.1 -n /cygdrive/c/Users/ronald/github/UhKc/ -a /cygdrive/c/Users/ronald/github/uh-kc-api/coeus-api-all</t>
   </si>
@@ -5813,12 +5815,451 @@
   <si>
     <t>coeus-impl/src/main/java/org/kuali/coeus/propdev/impl/approve/ProposalDevelopmentApproverViewAction.java</t>
   </si>
+  <si>
+    <t>kc_project/pom.xml</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/java/org/kuali/kra/bo/Rolodex.java</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/java/org/kuali/kra/bo/RolodexMaintainableImpl.java</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/java/org/kuali/kra/budget/nonpersonnel/BudgetLineItemBase.java</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/java/org/kuali/kra/budget/summary/BudgetSummaryServiceImpl.java</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/java/org/kuali/kra/questionnaire/answer/QuestionnaireAnswerServiceImpl.java</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/java/org/kuali/kra/web/struts/action/KraHoldingPageAction.java</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/resources/org/kuali/kra/datadictionary/Rolodex.xml</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/resources/org/kuali/kra/datadictionary/docs/RolodexMaintenanceDocument.xml</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/resources/org/kuali/kra/datadictionary/docs/SponsorSpecialMaintenanceDocument.xml</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/resources/repository.xml</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/webapp/WEB-INF/tags/questionnaire/questionnaireAnswersBody.tag</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/webapp/WEB-INF/tags/uh/leaveApplication.tag</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/webapp/WEB-INF/tags/uh/userHasRole.tag</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/webapp/WEB-INF/tags/uh/userIsAdmin.tag</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/webapp/WEB-INF/tags/uh/userLacksRole.tag</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/webapp/WEB-INF/tags/uh/userNotAdmin.tag</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/webapp/WEB-INF/tags/uh/workflowEnabledApps.tag</t>
+  </si>
+  <si>
+    <t>kc_project/src/main/webapp/scripts/questionnaireAnswer.js</t>
+  </si>
+  <si>
+    <t>File Altered</t>
+  </si>
+  <si>
+    <t>git command</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Diff Command</t>
+  </si>
+  <si>
+    <t>Modify rice version to UH version (we will need to do this later)
+exclude KualiLookup.jsp added
+KC-755 Remove Organization Lookup from Address Book (May no longer be needed.   We need to test Address Book entry to see if it requires organization. (Skiped)</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Not Merged</t>
+  </si>
+  <si>
+    <t>KC-755 Remove Organization Lookup already in KC6.0</t>
+  </si>
+  <si>
+    <t>Not Merged change in KC6.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KC-??? added patch from kuali.org released 4/19/2012 to prevent server crash when Get All Budget Periods is issued. </t>
+  </si>
+  <si>
+    <t>KC-803 Nested questions don't display correctly after save (Patch from KC 5.2.1)</t>
+  </si>
+  <si>
+    <t>KC-723 ... Pulling in 5.2 change to fix document close holding page issue</t>
+  </si>
+  <si>
+    <t>KC-563 ... Modifed fix to match Kuali fix KRACOEUS-6452</t>
+  </si>
+  <si>
+    <t>Not Merged file no longer exists and change wasn't needed</t>
+  </si>
+  <si>
+    <t>Leave Files don't belong in KC (added by Shaun in 2011)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of changed generated using </t>
+  </si>
+  <si>
+    <t>git diff --name-status master..community-releases   | cut -d$'\t'  -f2</t>
+  </si>
+  <si>
+    <t>d112314</t>
+  </si>
+  <si>
+    <t>Apply KC-742 Delegation lookups not working for Delegatee/Delegator during edit/add</t>
+  </si>
+  <si>
+    <t>19c64a9</t>
+  </si>
+  <si>
+    <t>Apply KC-715 Make document id the default focus on document search</t>
+  </si>
+  <si>
+    <t>c0f55ad</t>
+  </si>
+  <si>
+    <t>Apply KC-663 remove ad hoc action Request "Complete" options</t>
+  </si>
+  <si>
+    <t>66be3ec</t>
+  </si>
+  <si>
+    <t>Apply KC-652 fix for initiator receives incident report after attempting to recall proposal created in 3.x</t>
+  </si>
+  <si>
+    <t>2ab3ece</t>
+  </si>
+  <si>
+    <t>Apply KC-584 fix to use UH email reroute enhancement</t>
+  </si>
+  <si>
+    <t>b627c48</t>
+  </si>
+  <si>
+    <t>Apply fix Proposal Project Titles now visible to all via doc search</t>
+  </si>
+  <si>
+    <t>41daacf</t>
+  </si>
+  <si>
+    <t>Apply UH mod add UH number label for prncplId and remove search fields from Person Lookup</t>
+  </si>
+  <si>
+    <t>e9514c6</t>
+  </si>
+  <si>
+    <t>Apply uh mod to check for null (removed several from 8fa0e6309cd13e4e2369b1c691f92ea902b1a70d) which seemed unneccessary</t>
+  </si>
+  <si>
+    <t>9745b0d</t>
+  </si>
+  <si>
+    <t>Apply KC-427 When adding a delegation, the role of all other previously added delegations switches to the most recently added</t>
+  </si>
+  <si>
+    <t>4c8e613</t>
+  </si>
+  <si>
+    <t>Apply UH mod for KC-435 unable to open some attachments in IP docs</t>
+  </si>
+  <si>
+    <t>6d25de8</t>
+  </si>
+  <si>
+    <t>UH Constant changes (changed SYSTEM_USER from "kr" to "krsys"</t>
+  </si>
+  <si>
+    <t>36c66d3</t>
+  </si>
+  <si>
+    <t>Apply UH Mod change campus code length to 10 chars</t>
+  </si>
+  <si>
+    <t>bc4dbc9</t>
+  </si>
+  <si>
+    <t>Apply UH mod added new uh-config-defaults.xml which configures daily/weekly email crons</t>
+  </si>
+  <si>
+    <t>b9d6f53</t>
+  </si>
+  <si>
+    <t>Apply UH Mode for Logout action</t>
+  </si>
+  <si>
+    <t>99f020c</t>
+  </si>
+  <si>
+    <t>Apply KC-433, KC-623,KC-631,KC-618 Not Applying (KC-634, KC-638)</t>
+  </si>
+  <si>
+    <t>06eb8b8</t>
+  </si>
+  <si>
+    <t>change kr to krsys since kr is a real UH user name</t>
+  </si>
+  <si>
+    <t>477dd63</t>
+  </si>
+  <si>
+    <t>Apply UH performance improvement based on similar mod found in KULRICE-4070</t>
+  </si>
+  <si>
+    <t>6cec561</t>
+  </si>
+  <si>
+    <t>override email and encryption services with UH implementations</t>
+  </si>
+  <si>
+    <t>Commit SHA</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>GitK Command</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>db/impex/master/src/main/resources/KRIM_PRNCPL_T.xml</t>
+  </si>
+  <si>
+    <t>db/impex/server/bootstrap/src/main/resources/KRIM_PRNCPL_T.xml</t>
+  </si>
+  <si>
+    <t>db/impex/server/demo/src/main/resources/KRIM_PRNCPL_T.xml</t>
+  </si>
+  <si>
+    <t>rice-framework/krad-app-framework/src/main/java/org/kuali/rice/krad/util/KRADConstants.java</t>
+  </si>
+  <si>
+    <t>rice-framework/krad-service-impl/src/main/java/org/kuali/rice/krad/service/impl/AttachmentServiceImpl.java</t>
+  </si>
+  <si>
+    <t>rice-framework/krad-web-framework/src/main/resources/org/kuali/rice/krad/config/UHKRADOverrideSpringBeans.xml</t>
+  </si>
+  <si>
+    <t>rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/mo/common/active/InactivatableFromToUtils.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/util/xml/XmlHelper.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/encryption/AesEncryptor.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/encryption/UHEncryptionServiceImpl.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/mail/UHKualiExceptionIncidentServiceImpl.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/mail/UHStyleableEmailContentServiceImpl.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/struts/LogoutAction.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kcb/quartz/MessageProcessingJob.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/DocumentSearchCriteriaProcessorKEWAdapter.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/xml/XMLSearchableAttributeContent.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kew/doctype/service/impl/DocumentActionsPermissionBase.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kew/mail/service/impl/ActionListEmailServiceImpl.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kim/bo/ui/KimDocumentBoActivatableToFromEditableBase.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementKimDocument.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementPersonDocument.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementRoleDocument.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kim/service/impl/UiDocumentServiceImpl.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/java/org/kuali/rice/kim/web/struts/action/IdentityManagementPersonDocumentAction.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/resources/META-INF/uh-config-defaults.xml</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/resources/org/kuali/rice/kew/config/KewEmbeddedSpringBeans.xml.orig</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/resources/org/kuali/rice/kew/config/UHKEWOverrideSpringBeans.xml</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/resources/org/kuali/rice/kew/impl/document/search/DocumentSearchCriteriaBo.xml</t>
+  </si>
+  <si>
+    <t>rice-middleware/impl/src/main/resources/org/kuali/rice/kim/bo/datadictionary/PersonDocumentAffiliation.xml</t>
+  </si>
+  <si>
+    <t>rice-middleware/kew/api/src/main/java/org/kuali/rice/kew/api/KewApiConstants.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/kim/kim-impl/src/main/groovy/org/kuali/rice/kim/impl/common/active/ActiveFromToBo.groovy</t>
+  </si>
+  <si>
+    <t>rice-middleware/kim/kim-impl/src/main/resources/org/kuali/rice/kim/impl/identity/PersonImpl.xml</t>
+  </si>
+  <si>
+    <t>rice-middleware/kns/src/main/java/org/kuali/rice/kns/util/FieldUtils.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/kns/src/main/java/org/kuali/rice/kns/web/struts/action/KualiDocumentActionBase.java</t>
+  </si>
+  <si>
+    <t>rice-middleware/location/web/src/main/resources/org/kuali/rice/location/web/campus/Campus.xml</t>
+  </si>
+  <si>
+    <t>rice-middleware/web/src/main/webapp/WEB-INF/struts-config.xml</t>
+  </si>
+  <si>
+    <t>git list files</t>
+  </si>
+  <si>
+    <t>Found Count</t>
+  </si>
+  <si>
+    <t>Files Modified</t>
+  </si>
+  <si>
+    <t>Merge command</t>
+  </si>
+  <si>
+    <t>Base Rice Directory</t>
+  </si>
+  <si>
+    <t>UH Mod Directory</t>
+  </si>
+  <si>
+    <t>Rice 2.5.2 Directory</t>
+  </si>
+  <si>
+    <t>/cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/</t>
+  </si>
+  <si>
+    <t>/cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/</t>
+  </si>
+  <si>
+    <t>/cygdrive/c/Users/ronald/github/rice/</t>
+  </si>
+  <si>
+    <t>Action Taken</t>
+  </si>
+  <si>
+    <t>Removed- Junk file merged by accident….it's a merge orig file</t>
+  </si>
+  <si>
+    <t>Removed-Don't need this (acts on uh.bundled.rice property which we never set) must be something for profiler/travel/etc</t>
+  </si>
+  <si>
+    <t>Removed-another UH rice feature we are not using.  It sends exception emails to a list.  KC does then when the user asks and we never enabled this feature so dropping</t>
+  </si>
+  <si>
+    <t>Copied-Not sure if we use this….we should test and remove if not needed.</t>
+  </si>
+  <si>
+    <t>Copied but edited to remove the exception service</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>^
+^</t>
+  </si>
+  <si>
+    <t>^
+^
+^</t>
+  </si>
+  <si>
+    <t>Removed-Override to email which I don't think we use.</t>
+  </si>
+  <si>
+    <t>Removed KC 6.0 same code</t>
+  </si>
+  <si>
+    <t>Merged-Not really needed but can't hurt</t>
+  </si>
+  <si>
+    <t>Removed - Only change was a comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERGED-KC-623 When a role is added with an effective date in the future, the role does not show in the profile until the effective date.
+</t>
+  </si>
+  <si>
+    <t>Manually Merged - ActiveFromToBo.java (no longer groovy)</t>
+  </si>
+  <si>
+    <t>Not needed anymore titles no longer contain private data</t>
+  </si>
+  <si>
+    <t>We should test if this works now and if we like it.  My testing in Test Drive shows that it doesn't fail but it says user not authorized which makes it useless at this point.  So we should make this change.</t>
+  </si>
+  <si>
+    <t>Review-Not sure if logout is needed anymore since KC supports CAS now</t>
+  </si>
+  <si>
+    <t>merged KC-618</t>
+  </si>
+  <si>
+    <t>Not needed (cron setup for daily and weekly emails which we don’t use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merged
+KC-433 Show inactive delegations members so we can edit ???? Should we keep ?
+KC-631 Person Documents stuck enroute trying to edit if delegation exists.
+KC-618 fix incident report when adding delegations
+KC-623 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5954,8 +6395,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6147,6 +6594,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -6308,7 +6761,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -6329,6 +6782,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6666,8 +7131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="E123" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="12" topLeftCell="E195" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
       <selection pane="bottomRight" activeCell="M125" sqref="M125"/>
@@ -17873,4 +18338,1553 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="123.140625" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="13" customFormat="1">
+      <c r="A2" s="13" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1898</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>1900</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>1899</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75">
+      <c r="A3" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B3" s="12" t="str">
+        <f>CONCATENATE("gitk ",A3)</f>
+        <v>gitk kc_project/pom.xml</v>
+      </c>
+      <c r="C3" t="str">
+        <f>CONCATENATE("git difftool master..community-releases ",A3)</f>
+        <v>git difftool master..community-releases kc_project/pom.xml</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1901</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B4" s="12" t="str">
+        <f t="shared" ref="B4:B21" si="0">CONCATENATE("gitk ",A4)</f>
+        <v>gitk kc_project/src/main/java/org/kuali/kra/bo/Rolodex.java</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C21" si="1">CONCATENATE("git difftool master..community-releases ",A4)</f>
+        <v>git difftool master..community-releases kc_project/src/main/java/org/kuali/kra/bo/Rolodex.java</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1904</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B5" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/java/org/kuali/kra/bo/RolodexMaintainableImpl.java</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/java/org/kuali/kra/bo/RolodexMaintainableImpl.java</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1904</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/java/org/kuali/kra/budget/nonpersonnel/BudgetLineItemBase.java</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/java/org/kuali/kra/budget/nonpersonnel/BudgetLineItemBase.java</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>1906</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B7" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/java/org/kuali/kra/budget/summary/BudgetSummaryServiceImpl.java</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/java/org/kuali/kra/budget/summary/BudgetSummaryServiceImpl.java</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1906</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/java/org/kuali/kra/questionnaire/answer/QuestionnaireAnswerServiceImpl.java</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/java/org/kuali/kra/questionnaire/answer/QuestionnaireAnswerServiceImpl.java</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1907</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/java/org/kuali/kra/web/struts/action/KraHoldingPageAction.java</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/java/org/kuali/kra/web/struts/action/KraHoldingPageAction.java</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1908</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>1885</v>
+      </c>
+      <c r="B10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/resources/org/kuali/kra/datadictionary/Rolodex.xml</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/resources/org/kuali/kra/datadictionary/Rolodex.xml</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1904</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B11" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/resources/org/kuali/kra/datadictionary/docs/RolodexMaintenanceDocument.xml</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/resources/org/kuali/kra/datadictionary/docs/RolodexMaintenanceDocument.xml</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1904</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B12" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/resources/org/kuali/kra/datadictionary/docs/SponsorSpecialMaintenanceDocument.xml</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/resources/org/kuali/kra/datadictionary/docs/SponsorSpecialMaintenanceDocument.xml</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1909</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B13" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/resources/repository.xml</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/resources/repository.xml</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1904</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/webapp/WEB-INF/tags/questionnaire/questionnaireAnswersBody.tag</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/webapp/WEB-INF/tags/questionnaire/questionnaireAnswersBody.tag</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1907</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B15" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/webapp/WEB-INF/tags/uh/leaveApplication.tag</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/webapp/WEB-INF/tags/uh/leaveApplication.tag</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B16" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/webapp/WEB-INF/tags/uh/userHasRole.tag</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/webapp/WEB-INF/tags/uh/userHasRole.tag</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B17" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/webapp/WEB-INF/tags/uh/userIsAdmin.tag</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/webapp/WEB-INF/tags/uh/userIsAdmin.tag</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B18" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/webapp/WEB-INF/tags/uh/userLacksRole.tag</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/webapp/WEB-INF/tags/uh/userLacksRole.tag</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B19" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/webapp/WEB-INF/tags/uh/userNotAdmin.tag</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/webapp/WEB-INF/tags/uh/userNotAdmin.tag</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B20" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/webapp/WEB-INF/tags/uh/workflowEnabledApps.tag</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/webapp/WEB-INF/tags/uh/workflowEnabledApps.tag</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>1896</v>
+      </c>
+      <c r="B21" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>gitk kc_project/src/main/webapp/scripts/questionnaireAnswer.js</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>git difftool master..community-releases kc_project/src/main/webapp/scripts/questionnaireAnswer.js</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1907</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="118" customWidth="1"/>
+    <col min="5" max="5" width="60.140625" customWidth="1"/>
+    <col min="6" max="6" width="60.7109375" customWidth="1"/>
+    <col min="7" max="7" width="73.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="14" customFormat="1">
+      <c r="A5" s="14" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>1952</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>1990</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>2000</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>1951</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B6" t="str">
+        <f>CONCATENATE("gitk ",A6)</f>
+        <v>gitk d112314</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C13" si="0">CONCATENATE("git show --pretty=""format:"" --name-only ",A6)</f>
+        <v>git show --pretty="format:" --name-only d112314</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>1986</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1915</v>
+      </c>
+      <c r="G6" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D6," ",$B$2, D6, " ", $B$3,D6," ",$B$3,D6)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/kns/src/main/java/org/kuali/rice/kns/util/FieldUtils.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/kns/src/main/java/org/kuali/rice/kns/util/FieldUtils.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/kns/src/main/java/org/kuali/rice/kns/util/FieldUtils.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/kns/src/main/java/org/kuali/rice/kns/util/FieldUtils.java</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" ref="B7:B33" si="1">CONCATENATE("gitk ",A7)</f>
+        <v>gitk 19c64a9</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>git show --pretty="format:" --name-only 19c64a9</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>1968</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1917</v>
+      </c>
+      <c r="G7" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D7," ",$B$2, D7, " ", $B$3,D7," ",$B$3,D7)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/DocumentSearchCriteriaProcessorKEWAdapter.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/DocumentSearchCriteriaProcessorKEWAdapter.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/DocumentSearchCriteriaProcessorKEWAdapter.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/DocumentSearchCriteriaProcessorKEWAdapter.java</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60">
+      <c r="A8" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk c0f55ad</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>git show --pretty="format:" --name-only c0f55ad</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>1987</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>2016</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1919</v>
+      </c>
+      <c r="G8" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D8," ",$B$2, D8, " ", $B$3,D8," ",$B$3,D8)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/kns/src/main/java/org/kuali/rice/kns/web/struts/action/KualiDocumentActionBase.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/kns/src/main/java/org/kuali/rice/kns/web/struts/action/KualiDocumentActionBase.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/kns/src/main/java/org/kuali/rice/kns/web/struts/action/KualiDocumentActionBase.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/kns/src/main/java/org/kuali/rice/kns/web/struts/action/KualiDocumentActionBase.java</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 66be3ec</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>git show --pretty="format:" --name-only 66be3ec</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>1970</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1921</v>
+      </c>
+      <c r="G9" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D9," ",$B$2, D9, " ", $B$3,D9," ",$B$3,D9)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kew/doctype/service/impl/DocumentActionsPermissionBase.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kew/doctype/service/impl/DocumentActionsPermissionBase.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kew/doctype/service/impl/DocumentActionsPermissionBase.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kew/doctype/service/impl/DocumentActionsPermissionBase.java</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 2ab3ece</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>git show --pretty="format:" --name-only 2ab3ece</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1923</v>
+      </c>
+      <c r="G10" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D10," ",$B$2, D10, " ", $B$3,D10," ",$B$3,D10)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kew/mail/service/impl/ActionListEmailServiceImpl.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kew/mail/service/impl/ActionListEmailServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kew/mail/service/impl/ActionListEmailServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kew/mail/service/impl/ActionListEmailServiceImpl.java</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk b627c48</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>git show --pretty="format:" --name-only b627c48</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>1981</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2015</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1925</v>
+      </c>
+      <c r="G11" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D11," ",$B$2, D11, " ", $B$3,D11," ",$B$3,D11)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/impl/document/search/DocumentSearchCriteriaBo.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/impl/document/search/DocumentSearchCriteriaBo.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/impl/document/search/DocumentSearchCriteriaBo.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/impl/document/search/DocumentSearchCriteriaBo.xml</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 41daacf</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>git show --pretty="format:" --name-only 41daacf</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>1985</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1927</v>
+      </c>
+      <c r="G12" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D12," ",$B$2, D12, " ", $B$3,D12," ",$B$3,D12)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/kim/kim-impl/src/main/resources/org/kuali/rice/kim/impl/identity/PersonImpl.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/kim/kim-impl/src/main/resources/org/kuali/rice/kim/impl/identity/PersonImpl.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/kim/kim-impl/src/main/resources/org/kuali/rice/kim/impl/identity/PersonImpl.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/kim/kim-impl/src/main/resources/org/kuali/rice/kim/impl/identity/PersonImpl.xml</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk e9514c6</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>git show --pretty="format:" --name-only e9514c6</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>1967</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1929</v>
+      </c>
+      <c r="G13" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D13," ",$B$2, D13, " ", $B$3,D13," ",$B$3,D13)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kcb/quartz/MessageProcessingJob.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kcb/quartz/MessageProcessingJob.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kcb/quartz/MessageProcessingJob.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kcb/quartz/MessageProcessingJob.java</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>1930</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 9745b0d</v>
+      </c>
+      <c r="C14" t="str">
+        <f>CONCATENATE("git show --pretty=""format:"" --name-only ",A14)</f>
+        <v>git show --pretty="format:" --name-only 9745b0d</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>1973</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1931</v>
+      </c>
+      <c r="G14" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D14," ",$B$2, D14, " ", $B$3,D14," ",$B$3,D14)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementKimDocument.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementKimDocument.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementKimDocument.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementKimDocument.java</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="D15" s="16" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G15" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D15," ",$B$2, D15, " ", $B$3,D15," ",$B$3,D15)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementRoleDocument.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementRoleDocument.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementRoleDocument.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementRoleDocument.java</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 4c8e613</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" ref="C16:C33" si="2">CONCATENATE("git show --pretty=""format:"" --name-only ",A16)</f>
+        <v>git show --pretty="format:" --name-only 4c8e613</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>1958</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1933</v>
+      </c>
+      <c r="G16" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D16," ",$B$2, D16, " ", $B$3,D16," ",$B$3,D16)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-framework/krad-service-impl/src/main/java/org/kuali/rice/krad/service/impl/AttachmentServiceImpl.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-framework/krad-service-impl/src/main/java/org/kuali/rice/krad/service/impl/AttachmentServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-framework/krad-service-impl/src/main/java/org/kuali/rice/krad/service/impl/AttachmentServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-framework/krad-service-impl/src/main/java/org/kuali/rice/krad/service/impl/AttachmentServiceImpl.java</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 6d25de8</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="2"/>
+        <v>git show --pretty="format:" --name-only 6d25de8</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>1957</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1935</v>
+      </c>
+      <c r="G17" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D17," ",$B$2, D17, " ", $B$3,D17," ",$B$3,D17)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-framework/krad-app-framework/src/main/java/org/kuali/rice/krad/util/KRADConstants.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-framework/krad-app-framework/src/main/java/org/kuali/rice/krad/util/KRADConstants.java /cygdrive/c/Users/ronald/github/rice/rice-framework/krad-app-framework/src/main/java/org/kuali/rice/krad/util/KRADConstants.java /cygdrive/c/Users/ronald/github/rice/rice-framework/krad-app-framework/src/main/java/org/kuali/rice/krad/util/KRADConstants.java</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="D18" s="16" t="s">
+        <v>1983</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G18" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D18," ",$B$2, D18, " ", $B$3,D18," ",$B$3,D18)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/kew/api/src/main/java/org/kuali/rice/kew/api/KewApiConstants.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/kew/api/src/main/java/org/kuali/rice/kew/api/KewApiConstants.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/kew/api/src/main/java/org/kuali/rice/kew/api/KewApiConstants.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/kew/api/src/main/java/org/kuali/rice/kew/api/KewApiConstants.java</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>1936</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 36c66d3</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="2"/>
+        <v>git show --pretty="format:" --name-only 36c66d3</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>1982</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1937</v>
+      </c>
+      <c r="G19" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D19," ",$B$2, D19, " ", $B$3,D19," ",$B$3,D19)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/resources/org/kuali/rice/kim/bo/datadictionary/PersonDocumentAffiliation.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/resources/org/kuali/rice/kim/bo/datadictionary/PersonDocumentAffiliation.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/org/kuali/rice/kim/bo/datadictionary/PersonDocumentAffiliation.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/org/kuali/rice/kim/bo/datadictionary/PersonDocumentAffiliation.xml</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="D20" s="9" t="s">
+        <v>1988</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G20" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D20," ",$B$2, D20, " ", $B$3,D20," ",$B$3,D20)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/location/web/src/main/resources/org/kuali/rice/location/web/campus/Campus.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/location/web/src/main/resources/org/kuali/rice/location/web/campus/Campus.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/location/web/src/main/resources/org/kuali/rice/location/web/campus/Campus.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/location/web/src/main/resources/org/kuali/rice/location/web/campus/Campus.xml</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30">
+      <c r="A21" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk bc4dbc9</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="2"/>
+        <v>git show --pretty="format:" --name-only bc4dbc9</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>1978</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>2019</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1939</v>
+      </c>
+      <c r="G21" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D21," ",$B$2, D21, " ", $B$3,D21," ",$B$3,D21)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/resources/META-INF/uh-config-defaults.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/resources/META-INF/uh-config-defaults.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/META-INF/uh-config-defaults.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/META-INF/uh-config-defaults.xml</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 99f020c</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="2"/>
+        <v>git show --pretty="format:" --name-only 99f020c</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>1960</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1943</v>
+      </c>
+      <c r="G22" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D22," ",$B$2, D22, " ", $B$3,D22," ",$B$3,D22)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/mo/common/active/InactivatableFromToUtils.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/mo/common/active/InactivatableFromToUtils.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/mo/common/active/InactivatableFromToUtils.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/mo/common/active/InactivatableFromToUtils.java</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="D23" s="16" t="s">
+        <v>1972</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2018</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G23" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D23," ",$B$2, D23, " ", $B$3,D23," ",$B$3,D23)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kim/bo/ui/KimDocumentBoActivatableToFromEditableBase.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kim/bo/ui/KimDocumentBoActivatableToFromEditableBase.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/bo/ui/KimDocumentBoActivatableToFromEditableBase.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/bo/ui/KimDocumentBoActivatableToFromEditableBase.java</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="D24" s="16" t="s">
+        <v>1974</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>2012</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G24" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D24," ",$B$2, D24, " ", $B$3,D24," ",$B$3,D24)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementPersonDocument.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementPersonDocument.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementPersonDocument.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/document/IdentityManagementPersonDocument.java</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="D25" s="16" t="s">
+        <v>1976</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2020</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G25" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D25," ",$B$2, D25, " ", $B$3,D25," ",$B$3,D25)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kim/service/impl/UiDocumentServiceImpl.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kim/service/impl/UiDocumentServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/service/impl/UiDocumentServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/service/impl/UiDocumentServiceImpl.java</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="60">
+      <c r="D26" s="16" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>2013</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G26" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D26," ",$B$2, D26, " ", $B$3,D26," ",$B$3,D26)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kim/web/struts/action/IdentityManagementPersonDocumentAction.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kim/web/struts/action/IdentityManagementPersonDocumentAction.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/web/struts/action/IdentityManagementPersonDocumentAction.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kim/web/struts/action/IdentityManagementPersonDocumentAction.java</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="D27" s="16" t="s">
+        <v>1984</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>2014</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G27" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D27," ",$B$2, D27, " ", $B$3,D27," ",$B$3,D27)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/kim/kim-impl/src/main/groovy/org/kuali/rice/kim/impl/common/active/ActiveFromToBo.groovy /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/kim/kim-impl/src/main/groovy/org/kuali/rice/kim/impl/common/active/ActiveFromToBo.groovy /cygdrive/c/Users/ronald/github/rice/rice-middleware/kim/kim-impl/src/main/groovy/org/kuali/rice/kim/impl/common/active/ActiveFromToBo.groovy /cygdrive/c/Users/ronald/github/rice/rice-middleware/kim/kim-impl/src/main/groovy/org/kuali/rice/kim/impl/common/active/ActiveFromToBo.groovy</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 06eb8b8</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="2"/>
+        <v>git show --pretty="format:" --name-only 06eb8b8</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1954</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>2011</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1945</v>
+      </c>
+      <c r="G28" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D28," ",$B$2, D28, " ", $B$3,D28," ",$B$3,D28)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/db/impex/master/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/db/impex/master/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/github/rice/db/impex/master/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/github/rice/db/impex/master/src/main/resources/KRIM_PRNCPL_T.xml</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="D29" s="9" t="s">
+        <v>1955</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>2011</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G29" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D29," ",$B$2, D29, " ", $B$3,D29," ",$B$3,D29)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/db/impex/server/bootstrap/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/db/impex/server/bootstrap/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/github/rice/db/impex/server/bootstrap/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/github/rice/db/impex/server/bootstrap/src/main/resources/KRIM_PRNCPL_T.xml</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="D30" s="9" t="s">
+        <v>1956</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>2011</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G30" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D30," ",$B$2, D30, " ", $B$3,D30," ",$B$3,D30)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/db/impex/server/demo/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/db/impex/server/demo/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/github/rice/db/impex/server/demo/src/main/resources/KRIM_PRNCPL_T.xml /cygdrive/c/Users/ronald/github/rice/db/impex/server/demo/src/main/resources/KRIM_PRNCPL_T.xml</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 477dd63</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="2"/>
+        <v>git show --pretty="format:" --name-only 477dd63</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>1961</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>2010</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1947</v>
+      </c>
+      <c r="G31" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D31," ",$B$2, D31, " ", $B$3,D31," ",$B$3,D31)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/util/xml/XmlHelper.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/util/xml/XmlHelper.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/util/xml/XmlHelper.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/core/api/src/main/java/org/kuali/rice/core/api/util/xml/XmlHelper.java</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="D32" s="16" t="s">
+        <v>1969</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>2010</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G32" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D32," ",$B$2, D32, " ", $B$3,D32," ",$B$3,D32)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/xml/XMLSearchableAttributeContent.java /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/xml/XMLSearchableAttributeContent.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/xml/XMLSearchableAttributeContent.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/org/kuali/rice/kew/docsearch/xml/XMLSearchableAttributeContent.java</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="1"/>
+        <v>gitk 6cec561</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="2"/>
+        <v>git show --pretty="format:" --name-only 6cec561</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1959</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>2005</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1949</v>
+      </c>
+      <c r="G33" s="15" t="str">
+        <f>CONCATENATE("cp ",$B$2,D33," ",$B$3,D33)</f>
+        <v>cp /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-framework/krad-web-framework/src/main/resources/org/kuali/rice/krad/config/UHKRADOverrideSpringBeans.xml /cygdrive/c/Users/ronald/github/rice/rice-framework/krad-web-framework/src/main/resources/org/kuali/rice/krad/config/UHKRADOverrideSpringBeans.xml</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30">
+      <c r="D34" s="9" t="s">
+        <v>1962</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>2004</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>2007</v>
+      </c>
+      <c r="G34" s="15" t="str">
+        <f>CONCATENATE("cp ",$B$2,D34," ",$B$3,D34)</f>
+        <v>cp /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/encryption/AesEncryptor.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/encryption/AesEncryptor.java</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30">
+      <c r="D35" s="9" t="s">
+        <v>1963</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>2004</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>2007</v>
+      </c>
+      <c r="G35" s="15" t="str">
+        <f>CONCATENATE("cp ",$B$2,D35," ",$B$3,D35)</f>
+        <v>cp /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/encryption/UHEncryptionServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/encryption/UHEncryptionServiceImpl.java</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45">
+      <c r="D36" s="9" t="s">
+        <v>1964</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>2003</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>2008</v>
+      </c>
+      <c r="G36" s="15" t="str">
+        <f>CONCATENATE("cp ",$B$2,D36," ",$B$3,D36)</f>
+        <v>cp /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/mail/UHKualiExceptionIncidentServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/mail/UHKualiExceptionIncidentServiceImpl.java</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30">
+      <c r="D37" s="9" t="s">
+        <v>1965</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>2007</v>
+      </c>
+      <c r="G37" s="15" t="str">
+        <f>CONCATENATE("cp ",$B$2,D37," ",$B$3,D37)</f>
+        <v>cp /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/mail/UHStyleableEmailContentServiceImpl.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/mail/UHStyleableEmailContentServiceImpl.java</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30">
+      <c r="D38" s="9" t="s">
+        <v>1966</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>2017</v>
+      </c>
+      <c r="F38" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G38" s="15" t="str">
+        <f>CONCATENATE("cp ",$B$2,D38," ",$B$3,D38)</f>
+        <v>cp /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/struts/LogoutAction.java /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/java/edu/hawaii/its/kuali/struts/LogoutAction.java</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30">
+      <c r="A39" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B39" t="str">
+        <f>CONCATENATE("gitk ",A39)</f>
+        <v>gitk b9d6f53</v>
+      </c>
+      <c r="C39" t="str">
+        <f>CONCATENATE("git show --pretty=""format:"" --name-only ",A39)</f>
+        <v>git show --pretty="format:" --name-only b9d6f53</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>1989</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>2017</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1941</v>
+      </c>
+      <c r="G39" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D39," ",$B$2, D39, " ", $B$3,D39," ",$B$3,D39)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/web/src/main/webapp/WEB-INF/struts-config.xml /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/web/src/main/webapp/WEB-INF/struts-config.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/web/src/main/webapp/WEB-INF/struts-config.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/web/src/main/webapp/WEB-INF/struts-config.xml</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="D40" s="9" t="s">
+        <v>1979</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>2001</v>
+      </c>
+      <c r="F40" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G40" s="15" t="str">
+        <f>CONCATENATE("p4fix.sh ", $B$1, D40," ",$B$2, D40, " ", $B$3,D40," ",$B$3,D40)</f>
+        <v>p4fix.sh /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5.community/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/config/KewEmbeddedSpringBeans.xml.orig /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/config/KewEmbeddedSpringBeans.xml.orig /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/config/KewEmbeddedSpringBeans.xml.orig /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/config/KewEmbeddedSpringBeans.xml.orig</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="D41" s="9" t="s">
+        <v>1980</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>2009</v>
+      </c>
+      <c r="F41" t="s">
+        <v>2006</v>
+      </c>
+      <c r="G41" s="15" t="str">
+        <f>CONCATENATE("cp ",$B$2,D41," ",$B$3,D41)</f>
+        <v>cp /cygdrive/c/Users/ronald/uh-kc-rice-2.3.5/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/config/UHKEWOverrideSpringBeans.xml /cygdrive/c/Users/ronald/github/rice/rice-middleware/impl/src/main/resources/org/kuali/rice/kew/config/UHKEWOverrideSpringBeans.xml</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>1991</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B45,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B46,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B47,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B48,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B49,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1958</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B50,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B51,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B52,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B53,"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B54,"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B55,"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B56,"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B57,"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B58,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B59,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B60,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B61,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B62,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B63,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B64,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1973</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B65,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B66,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B67,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B68,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B69,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B70,"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B71,"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B72,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B73,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B74,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B75,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B76,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B77,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B78,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B79,"*"))</f>
+        <v>1</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <f>COUNTIF($D$6:$D$33,CONCATENATE("*",B80,"*"))</f>
+        <v>0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>